<commit_message>
Update list of to-be-tracked-flights
</commit_message>
<xml_diff>
--- a/flights.xlsx
+++ b/flights.xlsx
@@ -251,7 +251,7 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H35"/>
+  <dimension ref="A1:H65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -304,17 +304,17 @@
     <row r="2">
       <c r="A2" s="0" t="inlineStr">
         <is>
-          <t>f10</t>
+          <t>f1</t>
         </is>
       </c>
       <c r="B2" s="0" t="inlineStr">
         <is>
-          <t>27-09-2019</t>
+          <t>2019-10-24</t>
         </is>
       </c>
       <c r="C2" s="0" t="inlineStr">
         <is>
-          <t>Fri</t>
+          <t>Thu</t>
         </is>
       </c>
       <c r="D2" s="0" t="inlineStr">
@@ -324,7 +324,7 @@
       </c>
       <c r="E2" s="0" t="inlineStr">
         <is>
-          <t>Indigo-6E2625</t>
+          <t>6E2484</t>
         </is>
       </c>
       <c r="F2" s="0" t="inlineStr">
@@ -339,7 +339,7 @@
       </c>
       <c r="H2" s="0" t="inlineStr">
         <is>
-          <t>0025</t>
+          <t>2330</t>
         </is>
       </c>
     </row>
@@ -351,12 +351,12 @@
       </c>
       <c r="B3" s="0" t="inlineStr">
         <is>
-          <t>27-09-2019</t>
+          <t>2019-10-24</t>
         </is>
       </c>
       <c r="C3" s="0" t="inlineStr">
         <is>
-          <t>Fri</t>
+          <t>Thu</t>
         </is>
       </c>
       <c r="D3" s="0" t="inlineStr">
@@ -366,7 +366,7 @@
       </c>
       <c r="E3" s="0" t="inlineStr">
         <is>
-          <t>GoAir-G8118</t>
+          <t>SG8720</t>
         </is>
       </c>
       <c r="F3" s="0" t="inlineStr">
@@ -381,7 +381,7 @@
       </c>
       <c r="H3" s="0" t="inlineStr">
         <is>
-          <t>2055</t>
+          <t>2200</t>
         </is>
       </c>
     </row>
@@ -393,12 +393,12 @@
       </c>
       <c r="B4" s="0" t="inlineStr">
         <is>
-          <t>28-09-2019</t>
+          <t>2019-10-24</t>
         </is>
       </c>
       <c r="C4" s="0" t="inlineStr">
         <is>
-          <t>Sat</t>
+          <t>Thu</t>
         </is>
       </c>
       <c r="D4" s="0" t="inlineStr">
@@ -408,7 +408,7 @@
       </c>
       <c r="E4" s="0" t="inlineStr">
         <is>
-          <t>GoAir-G8118</t>
+          <t>G8118</t>
         </is>
       </c>
       <c r="F4" s="0" t="inlineStr">
@@ -435,12 +435,12 @@
       </c>
       <c r="B5" s="0" t="inlineStr">
         <is>
-          <t>28-09-2019</t>
+          <t>2019-10-24</t>
         </is>
       </c>
       <c r="C5" s="0" t="inlineStr">
         <is>
-          <t>Sat</t>
+          <t>Thu</t>
         </is>
       </c>
       <c r="D5" s="0" t="inlineStr">
@@ -450,7 +450,7 @@
       </c>
       <c r="E5" s="0" t="inlineStr">
         <is>
-          <t>SpiceJ-SG6638</t>
+          <t>AI173</t>
         </is>
       </c>
       <c r="F5" s="0" t="inlineStr">
@@ -465,7 +465,7 @@
       </c>
       <c r="H5" s="0" t="inlineStr">
         <is>
-          <t>2310</t>
+          <t>2105</t>
         </is>
       </c>
     </row>
@@ -477,12 +477,12 @@
       </c>
       <c r="B6" s="0" t="inlineStr">
         <is>
-          <t>3-10-2019</t>
+          <t>2019-10-25</t>
         </is>
       </c>
       <c r="C6" s="0" t="inlineStr">
         <is>
-          <t>Tue</t>
+          <t>Fri</t>
         </is>
       </c>
       <c r="D6" s="0" t="inlineStr">
@@ -492,22 +492,22 @@
       </c>
       <c r="E6" s="0" t="inlineStr">
         <is>
-          <t>GoAir-G8113</t>
+          <t>6E2484</t>
         </is>
       </c>
       <c r="F6" s="0" t="inlineStr">
         <is>
-          <t>Del</t>
+          <t>Blr</t>
         </is>
       </c>
       <c r="G6" s="0" t="inlineStr">
         <is>
-          <t>Blr</t>
+          <t>Del</t>
         </is>
       </c>
       <c r="H6" s="0" t="inlineStr">
         <is>
-          <t>0550</t>
+          <t>2330</t>
         </is>
       </c>
     </row>
@@ -519,12 +519,12 @@
       </c>
       <c r="B7" s="0" t="inlineStr">
         <is>
-          <t>3-10-2019</t>
+          <t>2019-10-25</t>
         </is>
       </c>
       <c r="C7" s="0" t="inlineStr">
         <is>
-          <t>Tue</t>
+          <t>Fri</t>
         </is>
       </c>
       <c r="D7" s="0" t="inlineStr">
@@ -534,22 +534,22 @@
       </c>
       <c r="E7" s="0" t="inlineStr">
         <is>
-          <t>AirIn-AI933</t>
+          <t>SG8720</t>
         </is>
       </c>
       <c r="F7" s="0" t="inlineStr">
         <is>
-          <t>Del</t>
+          <t>Blr</t>
         </is>
       </c>
       <c r="G7" s="0" t="inlineStr">
         <is>
-          <t>Blr</t>
+          <t>Del</t>
         </is>
       </c>
       <c r="H7" s="0" t="inlineStr">
         <is>
-          <t>0510</t>
+          <t>2200</t>
         </is>
       </c>
     </row>
@@ -561,7 +561,7 @@
       </c>
       <c r="B8" s="0" t="inlineStr">
         <is>
-          <t>4-10-2019</t>
+          <t>2019-10-25</t>
         </is>
       </c>
       <c r="C8" s="0" t="inlineStr">
@@ -576,7 +576,7 @@
       </c>
       <c r="E8" s="0" t="inlineStr">
         <is>
-          <t>Indigo-6E2808</t>
+          <t>G8118</t>
         </is>
       </c>
       <c r="F8" s="0" t="inlineStr">
@@ -591,7 +591,7 @@
       </c>
       <c r="H8" s="0" t="inlineStr">
         <is>
-          <t>1930</t>
+          <t>2055</t>
         </is>
       </c>
     </row>
@@ -603,7 +603,7 @@
       </c>
       <c r="B9" s="0" t="inlineStr">
         <is>
-          <t>4-10-2019</t>
+          <t>2019-10-25</t>
         </is>
       </c>
       <c r="C9" s="0" t="inlineStr">
@@ -618,7 +618,7 @@
       </c>
       <c r="E9" s="0" t="inlineStr">
         <is>
-          <t>SpiceJ-SG6638</t>
+          <t>AI173</t>
         </is>
       </c>
       <c r="F9" s="0" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="H9" s="0" t="inlineStr">
         <is>
-          <t>2310</t>
+          <t>2105</t>
         </is>
       </c>
     </row>
@@ -645,12 +645,12 @@
       </c>
       <c r="B10" s="0" t="inlineStr">
         <is>
-          <t>7-10-2019</t>
+          <t>2019-11-01</t>
         </is>
       </c>
       <c r="C10" s="0" t="inlineStr">
         <is>
-          <t>Mon</t>
+          <t>Fri</t>
         </is>
       </c>
       <c r="D10" s="0" t="inlineStr">
@@ -660,7 +660,7 @@
       </c>
       <c r="E10" s="0" t="inlineStr">
         <is>
-          <t>SpiceJ-SG198</t>
+          <t>6E2484</t>
         </is>
       </c>
       <c r="F10" s="0" t="inlineStr">
@@ -675,7 +675,7 @@
       </c>
       <c r="H10" s="0" t="inlineStr">
         <is>
-          <t>2045</t>
+          <t>2330</t>
         </is>
       </c>
     </row>
@@ -687,12 +687,12 @@
       </c>
       <c r="B11" s="0" t="inlineStr">
         <is>
-          <t>7-10-2019</t>
+          <t>2019-11-01</t>
         </is>
       </c>
       <c r="C11" s="0" t="inlineStr">
         <is>
-          <t>Mon</t>
+          <t>Fri</t>
         </is>
       </c>
       <c r="D11" s="0" t="inlineStr">
@@ -702,7 +702,7 @@
       </c>
       <c r="E11" s="0" t="inlineStr">
         <is>
-          <t>Indigo-6E2305</t>
+          <t>SG8720</t>
         </is>
       </c>
       <c r="F11" s="0" t="inlineStr">
@@ -717,7 +717,7 @@
       </c>
       <c r="H11" s="0" t="inlineStr">
         <is>
-          <t>2125</t>
+          <t>2200</t>
         </is>
       </c>
     </row>
@@ -729,12 +729,12 @@
       </c>
       <c r="B12" s="0" t="inlineStr">
         <is>
-          <t>9-10-2019</t>
+          <t>2019-11-01</t>
         </is>
       </c>
       <c r="C12" s="0" t="inlineStr">
         <is>
-          <t>Wed</t>
+          <t>Fri</t>
         </is>
       </c>
       <c r="D12" s="0" t="inlineStr">
@@ -744,22 +744,22 @@
       </c>
       <c r="E12" s="0" t="inlineStr">
         <is>
-          <t>Indigo-6E2042</t>
+          <t>G8118</t>
         </is>
       </c>
       <c r="F12" s="0" t="inlineStr">
         <is>
-          <t>Del</t>
+          <t>Blr</t>
         </is>
       </c>
       <c r="G12" s="0" t="inlineStr">
         <is>
-          <t>Blr</t>
+          <t>Del</t>
         </is>
       </c>
       <c r="H12" s="0" t="inlineStr">
         <is>
-          <t>0545</t>
+          <t>2055</t>
         </is>
       </c>
     </row>
@@ -771,12 +771,12 @@
       </c>
       <c r="B13" s="0" t="inlineStr">
         <is>
-          <t>9-10-2019</t>
+          <t>2019-11-01</t>
         </is>
       </c>
       <c r="C13" s="0" t="inlineStr">
         <is>
-          <t>Wed</t>
+          <t>Fri</t>
         </is>
       </c>
       <c r="D13" s="0" t="inlineStr">
@@ -786,22 +786,22 @@
       </c>
       <c r="E13" s="0" t="inlineStr">
         <is>
-          <t>GoAir-G8113</t>
+          <t>AI173</t>
         </is>
       </c>
       <c r="F13" s="0" t="inlineStr">
         <is>
-          <t>Del</t>
+          <t>Blr</t>
         </is>
       </c>
       <c r="G13" s="0" t="inlineStr">
         <is>
-          <t>Blr</t>
+          <t>Del</t>
         </is>
       </c>
       <c r="H13" s="0" t="inlineStr">
         <is>
-          <t>0550</t>
+          <t>2110</t>
         </is>
       </c>
     </row>
@@ -813,12 +813,12 @@
       </c>
       <c r="B14" s="0" t="inlineStr">
         <is>
-          <t>24-10-2019</t>
+          <t>2019-11-02</t>
         </is>
       </c>
       <c r="C14" s="0" t="inlineStr">
         <is>
-          <t>Fri</t>
+          <t>Sat</t>
         </is>
       </c>
       <c r="D14" s="0" t="inlineStr">
@@ -828,7 +828,7 @@
       </c>
       <c r="E14" s="0" t="inlineStr">
         <is>
-          <t>AirIn-AI587</t>
+          <t>6E2289</t>
         </is>
       </c>
       <c r="F14" s="0" t="inlineStr">
@@ -843,7 +843,7 @@
       </c>
       <c r="H14" s="0" t="inlineStr">
         <is>
-          <t>2200</t>
+          <t>2220</t>
         </is>
       </c>
     </row>
@@ -855,12 +855,12 @@
       </c>
       <c r="B15" s="0" t="inlineStr">
         <is>
-          <t>24-10-2019</t>
+          <t>2019-11-02</t>
         </is>
       </c>
       <c r="C15" s="0" t="inlineStr">
         <is>
-          <t>Fri</t>
+          <t>Sat</t>
         </is>
       </c>
       <c r="D15" s="0" t="inlineStr">
@@ -870,7 +870,7 @@
       </c>
       <c r="E15" s="0" t="inlineStr">
         <is>
-          <t>GoAir-G8118</t>
+          <t>SG8720</t>
         </is>
       </c>
       <c r="F15" s="0" t="inlineStr">
@@ -885,7 +885,7 @@
       </c>
       <c r="H15" s="0" t="inlineStr">
         <is>
-          <t>2055</t>
+          <t>2200</t>
         </is>
       </c>
     </row>
@@ -897,12 +897,12 @@
       </c>
       <c r="B16" s="0" t="inlineStr">
         <is>
-          <t>25-10-2019</t>
+          <t>2019-11-02</t>
         </is>
       </c>
       <c r="C16" s="0" t="inlineStr">
         <is>
-          <t>Fri</t>
+          <t>Sat</t>
         </is>
       </c>
       <c r="D16" s="0" t="inlineStr">
@@ -912,7 +912,7 @@
       </c>
       <c r="E16" s="0" t="inlineStr">
         <is>
-          <t>GoAir-G8518</t>
+          <t>G8118</t>
         </is>
       </c>
       <c r="F16" s="0" t="inlineStr">
@@ -927,7 +927,7 @@
       </c>
       <c r="H16" s="0" t="inlineStr">
         <is>
-          <t>2255</t>
+          <t>2055</t>
         </is>
       </c>
     </row>
@@ -939,12 +939,12 @@
       </c>
       <c r="B17" s="0" t="inlineStr">
         <is>
-          <t>25-10-2019</t>
+          <t>2019-11-02</t>
         </is>
       </c>
       <c r="C17" s="0" t="inlineStr">
         <is>
-          <t>Fri</t>
+          <t>Sat</t>
         </is>
       </c>
       <c r="D17" s="0" t="inlineStr">
@@ -954,7 +954,7 @@
       </c>
       <c r="E17" s="0" t="inlineStr">
         <is>
-          <t>Indigo-6E2716</t>
+          <t>AI173</t>
         </is>
       </c>
       <c r="F17" s="0" t="inlineStr">
@@ -969,7 +969,7 @@
       </c>
       <c r="H17" s="0" t="inlineStr">
         <is>
-          <t>2000</t>
+          <t>2110</t>
         </is>
       </c>
     </row>
@@ -981,12 +981,12 @@
       </c>
       <c r="B18" s="0" t="inlineStr">
         <is>
-          <t>29-10-2019</t>
+          <t>2019-10-28</t>
         </is>
       </c>
       <c r="C18" s="0" t="inlineStr">
         <is>
-          <t>Fri</t>
+          <t>Mon</t>
         </is>
       </c>
       <c r="D18" s="0" t="inlineStr">
@@ -996,7 +996,7 @@
       </c>
       <c r="E18" s="0" t="inlineStr">
         <is>
-          <t>Indigo-6E5031</t>
+          <t>6E2624</t>
         </is>
       </c>
       <c r="F18" s="0" t="inlineStr">
@@ -1011,7 +1011,7 @@
       </c>
       <c r="H18" s="0" t="inlineStr">
         <is>
-          <t>0505</t>
+          <t>0200</t>
         </is>
       </c>
     </row>
@@ -1023,12 +1023,12 @@
       </c>
       <c r="B19" s="0" t="inlineStr">
         <is>
-          <t>29-10-2019</t>
+          <t>2019-10-28</t>
         </is>
       </c>
       <c r="C19" s="0" t="inlineStr">
         <is>
-          <t>Fri</t>
+          <t>Mon</t>
         </is>
       </c>
       <c r="D19" s="0" t="inlineStr">
@@ -1038,7 +1038,7 @@
       </c>
       <c r="E19" s="0" t="inlineStr">
         <is>
-          <t>AirIn-AI933</t>
+          <t>SG191</t>
         </is>
       </c>
       <c r="F19" s="0" t="inlineStr">
@@ -1053,7 +1053,7 @@
       </c>
       <c r="H19" s="0" t="inlineStr">
         <is>
-          <t>0510</t>
+          <t>0620</t>
         </is>
       </c>
     </row>
@@ -1065,12 +1065,12 @@
       </c>
       <c r="B20" s="0" t="inlineStr">
         <is>
-          <t>30-10-2019</t>
+          <t>2019-10-28</t>
         </is>
       </c>
       <c r="C20" s="0" t="inlineStr">
         <is>
-          <t>Fri</t>
+          <t>Mon</t>
         </is>
       </c>
       <c r="D20" s="0" t="inlineStr">
@@ -1080,7 +1080,7 @@
       </c>
       <c r="E20" s="0" t="inlineStr">
         <is>
-          <t>Indigo-6E2701</t>
+          <t>G8113</t>
         </is>
       </c>
       <c r="F20" s="0" t="inlineStr">
@@ -1095,7 +1095,7 @@
       </c>
       <c r="H20" s="0" t="inlineStr">
         <is>
-          <t>0655</t>
+          <t>0550</t>
         </is>
       </c>
     </row>
@@ -1107,12 +1107,12 @@
       </c>
       <c r="B21" s="0" t="inlineStr">
         <is>
-          <t>30-10-2019</t>
+          <t>2019-10-28</t>
         </is>
       </c>
       <c r="C21" s="0" t="inlineStr">
         <is>
-          <t>Fri</t>
+          <t>Mon</t>
         </is>
       </c>
       <c r="D21" s="0" t="inlineStr">
@@ -1122,7 +1122,7 @@
       </c>
       <c r="E21" s="0" t="inlineStr">
         <is>
-          <t>GoAir-G8207</t>
+          <t>AI803</t>
         </is>
       </c>
       <c r="F21" s="0" t="inlineStr">
@@ -1137,7 +1137,7 @@
       </c>
       <c r="H21" s="0" t="inlineStr">
         <is>
-          <t>0500</t>
+          <t>0610</t>
         </is>
       </c>
     </row>
@@ -1149,22 +1149,22 @@
       </c>
       <c r="B22" s="0" t="inlineStr">
         <is>
-          <t>25-09-2019</t>
+          <t>2019-10-29</t>
         </is>
       </c>
       <c r="C22" s="0" t="inlineStr">
         <is>
-          <t>Wed</t>
+          <t>Tue</t>
         </is>
       </c>
       <c r="D22" s="0" t="inlineStr">
         <is>
-          <t>Normal</t>
+          <t>Around Holiday</t>
         </is>
       </c>
       <c r="E22" s="0" t="inlineStr">
         <is>
-          <t>Indigo-6E5031</t>
+          <t>6E5031</t>
         </is>
       </c>
       <c r="F22" s="0" t="inlineStr">
@@ -1191,22 +1191,22 @@
       </c>
       <c r="B23" s="0" t="inlineStr">
         <is>
-          <t>25-09-2019</t>
+          <t>2019-10-29</t>
         </is>
       </c>
       <c r="C23" s="0" t="inlineStr">
         <is>
-          <t>Wed</t>
+          <t>Tue</t>
         </is>
       </c>
       <c r="D23" s="0" t="inlineStr">
         <is>
-          <t>Normal</t>
+          <t>Around Holiday</t>
         </is>
       </c>
       <c r="E23" s="0" t="inlineStr">
         <is>
-          <t>AirIn-AI851</t>
+          <t>SG191</t>
         </is>
       </c>
       <c r="F23" s="0" t="inlineStr">
@@ -1221,7 +1221,7 @@
       </c>
       <c r="H23" s="0" t="inlineStr">
         <is>
-          <t>0455</t>
+          <t>0620</t>
         </is>
       </c>
     </row>
@@ -1233,37 +1233,37 @@
       </c>
       <c r="B24" s="0" t="inlineStr">
         <is>
-          <t>25-09-2019</t>
+          <t>2019-10-29</t>
         </is>
       </c>
       <c r="C24" s="0" t="inlineStr">
         <is>
-          <t>Wed</t>
+          <t>Tue</t>
         </is>
       </c>
       <c r="D24" s="0" t="inlineStr">
         <is>
-          <t>Normal</t>
+          <t>Around Holiday</t>
         </is>
       </c>
       <c r="E24" s="0" t="inlineStr">
         <is>
-          <t>GoAir-G8518</t>
+          <t>G8113</t>
         </is>
       </c>
       <c r="F24" s="0" t="inlineStr">
         <is>
-          <t>Blr</t>
+          <t>Del</t>
         </is>
       </c>
       <c r="G24" s="0" t="inlineStr">
         <is>
-          <t>Del</t>
+          <t>Blr</t>
         </is>
       </c>
       <c r="H24" s="0" t="inlineStr">
         <is>
-          <t>2255</t>
+          <t>0550</t>
         </is>
       </c>
     </row>
@@ -1275,37 +1275,37 @@
       </c>
       <c r="B25" s="0" t="inlineStr">
         <is>
-          <t>25-09-2019</t>
+          <t>2019-10-29</t>
         </is>
       </c>
       <c r="C25" s="0" t="inlineStr">
         <is>
-          <t>Wed</t>
+          <t>Tue</t>
         </is>
       </c>
       <c r="D25" s="0" t="inlineStr">
         <is>
-          <t>Normal</t>
+          <t>Around Holiday</t>
         </is>
       </c>
       <c r="E25" s="0" t="inlineStr">
         <is>
-          <t>Indigo-6E2716</t>
+          <t>AI803</t>
         </is>
       </c>
       <c r="F25" s="0" t="inlineStr">
         <is>
-          <t>Blr</t>
+          <t>Del</t>
         </is>
       </c>
       <c r="G25" s="0" t="inlineStr">
         <is>
-          <t>Del</t>
+          <t>Blr</t>
         </is>
       </c>
       <c r="H25" s="0" t="inlineStr">
         <is>
-          <t>2000</t>
+          <t>0610</t>
         </is>
       </c>
     </row>
@@ -1317,7 +1317,7 @@
       </c>
       <c r="B26" s="0" t="inlineStr">
         <is>
-          <t>10-10-2019</t>
+          <t>2019-10-30</t>
         </is>
       </c>
       <c r="C26" s="0" t="inlineStr">
@@ -1327,27 +1327,27 @@
       </c>
       <c r="D26" s="0" t="inlineStr">
         <is>
-          <t>Normal</t>
+          <t>Around Holiday</t>
         </is>
       </c>
       <c r="E26" s="0" t="inlineStr">
         <is>
-          <t>SpiceJ-SG8720</t>
+          <t>6E503</t>
         </is>
       </c>
       <c r="F26" s="0" t="inlineStr">
         <is>
-          <t>Blr</t>
+          <t>Del</t>
         </is>
       </c>
       <c r="G26" s="0" t="inlineStr">
         <is>
-          <t>Del</t>
+          <t>Blr</t>
         </is>
       </c>
       <c r="H26" s="0" t="inlineStr">
         <is>
-          <t>2200</t>
+          <t>0505</t>
         </is>
       </c>
     </row>
@@ -1359,7 +1359,7 @@
       </c>
       <c r="B27" s="0" t="inlineStr">
         <is>
-          <t>10-10-2019</t>
+          <t>2019-10-30</t>
         </is>
       </c>
       <c r="C27" s="0" t="inlineStr">
@@ -1369,27 +1369,27 @@
       </c>
       <c r="D27" s="0" t="inlineStr">
         <is>
-          <t>Normal</t>
+          <t>Around Holiday</t>
         </is>
       </c>
       <c r="E27" s="0" t="inlineStr">
         <is>
-          <t>GoAir-G8118</t>
+          <t>SG191</t>
         </is>
       </c>
       <c r="F27" s="0" t="inlineStr">
         <is>
-          <t>Blr</t>
+          <t>Del</t>
         </is>
       </c>
       <c r="G27" s="0" t="inlineStr">
         <is>
-          <t>Del</t>
+          <t>Blr</t>
         </is>
       </c>
       <c r="H27" s="0" t="inlineStr">
         <is>
-          <t>2055</t>
+          <t>0620</t>
         </is>
       </c>
     </row>
@@ -1401,7 +1401,7 @@
       </c>
       <c r="B28" s="0" t="inlineStr">
         <is>
-          <t>10-10-2019</t>
+          <t>2019-10-30</t>
         </is>
       </c>
       <c r="C28" s="0" t="inlineStr">
@@ -1411,12 +1411,12 @@
       </c>
       <c r="D28" s="0" t="inlineStr">
         <is>
-          <t>Normal</t>
+          <t>Around Holiday</t>
         </is>
       </c>
       <c r="E28" s="0" t="inlineStr">
         <is>
-          <t>Indigo-6E683</t>
+          <t>G8113</t>
         </is>
       </c>
       <c r="F28" s="0" t="inlineStr">
@@ -1431,7 +1431,7 @@
       </c>
       <c r="H28" s="0" t="inlineStr">
         <is>
-          <t>0735</t>
+          <t>0550</t>
         </is>
       </c>
     </row>
@@ -1443,7 +1443,7 @@
       </c>
       <c r="B29" s="0" t="inlineStr">
         <is>
-          <t>10-10-2019</t>
+          <t>2019-10-30</t>
         </is>
       </c>
       <c r="C29" s="0" t="inlineStr">
@@ -1453,12 +1453,12 @@
       </c>
       <c r="D29" s="0" t="inlineStr">
         <is>
-          <t>Normal</t>
+          <t>Around Holiday</t>
         </is>
       </c>
       <c r="E29" s="0" t="inlineStr">
         <is>
-          <t>GoAir-G82610</t>
+          <t>AI803</t>
         </is>
       </c>
       <c r="F29" s="0" t="inlineStr">
@@ -1473,7 +1473,7 @@
       </c>
       <c r="H29" s="0" t="inlineStr">
         <is>
-          <t>0810</t>
+          <t>0610</t>
         </is>
       </c>
     </row>
@@ -1485,22 +1485,22 @@
       </c>
       <c r="B30" s="0" t="inlineStr">
         <is>
-          <t>7-11-2019</t>
+          <t>2019-11-04</t>
         </is>
       </c>
       <c r="C30" s="0" t="inlineStr">
         <is>
-          <t>Thu</t>
+          <t>Mon</t>
         </is>
       </c>
       <c r="D30" s="0" t="inlineStr">
         <is>
-          <t>Normal</t>
+          <t>Around Holiday</t>
         </is>
       </c>
       <c r="E30" s="0" t="inlineStr">
         <is>
-          <t>Indigo-6E5031</t>
+          <t>6E2134</t>
         </is>
       </c>
       <c r="F30" s="0" t="inlineStr">
@@ -1515,7 +1515,7 @@
       </c>
       <c r="H30" s="0" t="inlineStr">
         <is>
-          <t>0505</t>
+          <t>0305</t>
         </is>
       </c>
     </row>
@@ -1527,22 +1527,22 @@
       </c>
       <c r="B31" s="0" t="inlineStr">
         <is>
-          <t>7-11-2019</t>
+          <t>2019-11-04</t>
         </is>
       </c>
       <c r="C31" s="0" t="inlineStr">
         <is>
-          <t>Thu</t>
+          <t>Mon</t>
         </is>
       </c>
       <c r="D31" s="0" t="inlineStr">
         <is>
-          <t>Normal</t>
+          <t>Around Holiday</t>
         </is>
       </c>
       <c r="E31" s="0" t="inlineStr">
         <is>
-          <t>AirIn-AI933</t>
+          <t>SG191</t>
         </is>
       </c>
       <c r="F31" s="0" t="inlineStr">
@@ -1557,7 +1557,7 @@
       </c>
       <c r="H31" s="0" t="inlineStr">
         <is>
-          <t>0510</t>
+          <t>0620</t>
         </is>
       </c>
     </row>
@@ -1569,37 +1569,37 @@
       </c>
       <c r="B32" s="0" t="inlineStr">
         <is>
-          <t>7-11-2019</t>
+          <t>2019-11-04</t>
         </is>
       </c>
       <c r="C32" s="0" t="inlineStr">
         <is>
-          <t>Thu</t>
+          <t>Mon</t>
         </is>
       </c>
       <c r="D32" s="0" t="inlineStr">
         <is>
-          <t>Normal</t>
+          <t>Around Holiday</t>
         </is>
       </c>
       <c r="E32" s="0" t="inlineStr">
         <is>
-          <t>Indigo-6E2484</t>
+          <t>G8113</t>
         </is>
       </c>
       <c r="F32" s="0" t="inlineStr">
         <is>
-          <t>Blr</t>
+          <t>Del</t>
         </is>
       </c>
       <c r="G32" s="0" t="inlineStr">
         <is>
-          <t>Del</t>
+          <t>Blr</t>
         </is>
       </c>
       <c r="H32" s="0" t="inlineStr">
         <is>
-          <t>2330</t>
+          <t>0550</t>
         </is>
       </c>
     </row>
@@ -1611,54 +1611,54 @@
       </c>
       <c r="B33" s="0" t="inlineStr">
         <is>
-          <t>7-11-2019</t>
+          <t>2019-11-04</t>
         </is>
       </c>
       <c r="C33" s="0" t="inlineStr">
         <is>
-          <t>Thu</t>
+          <t>Mon</t>
         </is>
       </c>
       <c r="D33" s="0" t="inlineStr">
         <is>
-          <t>Normal</t>
+          <t>Around Holiday</t>
         </is>
       </c>
       <c r="E33" s="0" t="inlineStr">
         <is>
-          <t>AirIn-AI610</t>
+          <t>AI803</t>
         </is>
       </c>
       <c r="F33" s="0" t="inlineStr">
         <is>
-          <t>Blr</t>
+          <t>Del</t>
         </is>
       </c>
       <c r="G33" s="0" t="inlineStr">
         <is>
-          <t>Del</t>
+          <t>Blr</t>
         </is>
       </c>
       <c r="H33" s="0" t="inlineStr">
         <is>
-          <t>1910</t>
+          <t>0610</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0" t="inlineStr">
         <is>
-          <t>f31</t>
+          <t>f33</t>
         </is>
       </c>
       <c r="B34" s="0" t="inlineStr">
         <is>
-          <t>7-11-2019</t>
+          <t>2019-10-23</t>
         </is>
       </c>
       <c r="C34" s="0" t="inlineStr">
         <is>
-          <t>Thu</t>
+          <t>Wed</t>
         </is>
       </c>
       <c r="D34" s="0" t="inlineStr">
@@ -1668,7 +1668,7 @@
       </c>
       <c r="E34" s="0" t="inlineStr">
         <is>
-          <t>Indigo-6E2484</t>
+          <t>6E2484</t>
         </is>
       </c>
       <c r="F34" s="0" t="inlineStr">
@@ -1690,42 +1690,1302 @@
     <row r="35">
       <c r="A35" s="0" t="inlineStr">
         <is>
-          <t>f32</t>
+          <t>f34</t>
         </is>
       </c>
       <c r="B35" s="0" t="inlineStr">
         <is>
-          <t>7-11-2019</t>
+          <t>2019-10-23</t>
         </is>
       </c>
       <c r="C35" s="0" t="inlineStr">
         <is>
+          <t>Wed</t>
+        </is>
+      </c>
+      <c r="D35" s="0" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="E35" s="0" t="inlineStr">
+        <is>
+          <t>SG8906</t>
+        </is>
+      </c>
+      <c r="F35" s="0" t="inlineStr">
+        <is>
+          <t>Blr</t>
+        </is>
+      </c>
+      <c r="G35" s="0" t="inlineStr">
+        <is>
+          <t>Del</t>
+        </is>
+      </c>
+      <c r="H35" s="0" t="inlineStr">
+        <is>
+          <t>2310</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>f35</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>2019-10-23</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Wed</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>G8118</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>Blr</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>Del</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>2055</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>f36</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>2019-10-23</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Wed</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>AI173</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>Blr</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>Del</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>2105</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>f37</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>2019-10-24</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
           <t>Thu</t>
         </is>
       </c>
-      <c r="D35" s="0" t="inlineStr">
-        <is>
-          <t>Normal</t>
-        </is>
-      </c>
-      <c r="E35" s="0" t="inlineStr">
-        <is>
-          <t>AirIn-AI610</t>
-        </is>
-      </c>
-      <c r="F35" s="0" t="inlineStr">
-        <is>
-          <t>Blr</t>
-        </is>
-      </c>
-      <c r="G35" s="0" t="inlineStr">
-        <is>
-          <t>Del</t>
-        </is>
-      </c>
-      <c r="H35" s="0" t="inlineStr">
-        <is>
-          <t>1910</t>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>6E2484</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>Blr</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>Del</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>2330</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>f38</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>2019-10-24</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Thu</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>SG8720</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>Blr</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>Del</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>2200</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>f39</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>2019-10-24</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Thu</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>G8118</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>Blr</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>Del</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>2055</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>f40</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>2019-10-24</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Thu</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>AI173</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>Blr</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>Del</t>
+        </is>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>2105</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>f41</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>2019-11-06</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Wed</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>6E2484</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>Blr</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>Del</t>
+        </is>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>2330</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>f42</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>2019-11-06</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Wed</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>SG8720</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>Blr</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>Del</t>
+        </is>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>2200</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>f43</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>2019-11-06</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Wed</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>G8120</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>Blr</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>Del</t>
+        </is>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>1140</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>f44</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>2019-11-06</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Wed</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>AI173</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>Blr</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>Del</t>
+        </is>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>2110</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>f45</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>2019-09-07</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Thu</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>6E2484</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>Blr</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>Del</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>2330</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>f46</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>2019-09-07</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Thu</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>SG8720</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>Blr</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>Del</t>
+        </is>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>2200</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>f47</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>2019-09-07</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Thu</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>G8120</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>Blr</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>Del</t>
+        </is>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>1140</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>f48</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>2019-09-07</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Thu</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>AI173</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>Blr</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>Del</t>
+        </is>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>2110</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>f49</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>2019-10-23</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Wed</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>6E2458</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>Del</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>Blr</t>
+        </is>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>0625</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>f50</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>2019-10-23</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Wed</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>SG191</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>Del</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>Blr</t>
+        </is>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>0610</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>f51</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>2019-10-23</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Wed</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>G8113</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>Del</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>Blr</t>
+        </is>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>0550</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>f52</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>2019-10-23</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Wed</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>AI803</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>Del</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>Blr</t>
+        </is>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>0610</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>f53</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>2019-10-24</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Thu</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>6E5031</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>Del</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>Blr</t>
+        </is>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>0505</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>f54</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>2019-10-24</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>Thu</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>SG191</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>Del</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>Blr</t>
+        </is>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>0610</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>f55</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>2019-10-24</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Thu</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>G8113</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>Del</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>Blr</t>
+        </is>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>0550</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>f56</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>2019-10-24</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Thu</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>AI803</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>Del</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>Blr</t>
+        </is>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>0610</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>f57</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>2019-11-06</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Wed</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>6E2134</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>Del</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>Blr</t>
+        </is>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>0305</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>f58</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>2019-11-06</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Wed</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>SG191</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>Del</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>Blr</t>
+        </is>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>0620</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>f59</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>2019-11-06</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Wed</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>G8113</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>Del</t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>Blr</t>
+        </is>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>0505</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>f60</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>2019-11-06</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>Wed</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>AI803</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>Del</t>
+        </is>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>Blr</t>
+        </is>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>0610</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>f61</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>2019-11-07</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>Thu</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>6E5015</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>Del</t>
+        </is>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>Blr</t>
+        </is>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>0755</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>f62</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>2019-11-07</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>Thu</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>SG191</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>Del</t>
+        </is>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>Blr</t>
+        </is>
+      </c>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>0620</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>f63</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>2019-11-07</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>Thu</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>G8113</t>
+        </is>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>Del</t>
+        </is>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>Blr</t>
+        </is>
+      </c>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>0550</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>f64</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>2019-11-07</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>Thu</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>AI803</t>
+        </is>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>Del</t>
+        </is>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>Blr</t>
+        </is>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>0610</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Solves the issue of not enough time for JS to load
</commit_message>
<xml_diff>
--- a/flights.xlsx
+++ b/flights.xlsx
@@ -329,12 +329,12 @@
       </c>
       <c r="F2" s="0" t="inlineStr">
         <is>
-          <t>Blr</t>
+          <t>BLR</t>
         </is>
       </c>
       <c r="G2" s="0" t="inlineStr">
         <is>
-          <t>Del</t>
+          <t>DEL</t>
         </is>
       </c>
       <c r="H2" s="0" t="inlineStr">
@@ -371,12 +371,12 @@
       </c>
       <c r="F3" s="0" t="inlineStr">
         <is>
-          <t>Blr</t>
+          <t>BLR</t>
         </is>
       </c>
       <c r="G3" s="0" t="inlineStr">
         <is>
-          <t>Del</t>
+          <t>DEL</t>
         </is>
       </c>
       <c r="H3" s="0" t="inlineStr">
@@ -413,12 +413,12 @@
       </c>
       <c r="F4" s="0" t="inlineStr">
         <is>
-          <t>Blr</t>
+          <t>BLR</t>
         </is>
       </c>
       <c r="G4" s="0" t="inlineStr">
         <is>
-          <t>Del</t>
+          <t>DEL</t>
         </is>
       </c>
       <c r="H4" s="0" t="inlineStr">
@@ -455,12 +455,12 @@
       </c>
       <c r="F5" s="0" t="inlineStr">
         <is>
-          <t>Blr</t>
+          <t>BLR</t>
         </is>
       </c>
       <c r="G5" s="0" t="inlineStr">
         <is>
-          <t>Del</t>
+          <t>DEL</t>
         </is>
       </c>
       <c r="H5" s="0" t="inlineStr">
@@ -497,12 +497,12 @@
       </c>
       <c r="F6" s="0" t="inlineStr">
         <is>
-          <t>Blr</t>
+          <t>BLR</t>
         </is>
       </c>
       <c r="G6" s="0" t="inlineStr">
         <is>
-          <t>Del</t>
+          <t>DEL</t>
         </is>
       </c>
       <c r="H6" s="0" t="inlineStr">
@@ -539,12 +539,12 @@
       </c>
       <c r="F7" s="0" t="inlineStr">
         <is>
-          <t>Blr</t>
+          <t>BLR</t>
         </is>
       </c>
       <c r="G7" s="0" t="inlineStr">
         <is>
-          <t>Del</t>
+          <t>DEL</t>
         </is>
       </c>
       <c r="H7" s="0" t="inlineStr">
@@ -581,12 +581,12 @@
       </c>
       <c r="F8" s="0" t="inlineStr">
         <is>
-          <t>Blr</t>
+          <t>BLR</t>
         </is>
       </c>
       <c r="G8" s="0" t="inlineStr">
         <is>
-          <t>Del</t>
+          <t>DEL</t>
         </is>
       </c>
       <c r="H8" s="0" t="inlineStr">
@@ -623,12 +623,12 @@
       </c>
       <c r="F9" s="0" t="inlineStr">
         <is>
-          <t>Blr</t>
+          <t>BLR</t>
         </is>
       </c>
       <c r="G9" s="0" t="inlineStr">
         <is>
-          <t>Del</t>
+          <t>DEL</t>
         </is>
       </c>
       <c r="H9" s="0" t="inlineStr">
@@ -665,12 +665,12 @@
       </c>
       <c r="F10" s="0" t="inlineStr">
         <is>
-          <t>Blr</t>
+          <t>BLR</t>
         </is>
       </c>
       <c r="G10" s="0" t="inlineStr">
         <is>
-          <t>Del</t>
+          <t>DEL</t>
         </is>
       </c>
       <c r="H10" s="0" t="inlineStr">
@@ -707,12 +707,12 @@
       </c>
       <c r="F11" s="0" t="inlineStr">
         <is>
-          <t>Blr</t>
+          <t>BLR</t>
         </is>
       </c>
       <c r="G11" s="0" t="inlineStr">
         <is>
-          <t>Del</t>
+          <t>DEL</t>
         </is>
       </c>
       <c r="H11" s="0" t="inlineStr">
@@ -749,12 +749,12 @@
       </c>
       <c r="F12" s="0" t="inlineStr">
         <is>
-          <t>Blr</t>
+          <t>BLR</t>
         </is>
       </c>
       <c r="G12" s="0" t="inlineStr">
         <is>
-          <t>Del</t>
+          <t>DEL</t>
         </is>
       </c>
       <c r="H12" s="0" t="inlineStr">
@@ -791,12 +791,12 @@
       </c>
       <c r="F13" s="0" t="inlineStr">
         <is>
-          <t>Blr</t>
+          <t>BLR</t>
         </is>
       </c>
       <c r="G13" s="0" t="inlineStr">
         <is>
-          <t>Del</t>
+          <t>DEL</t>
         </is>
       </c>
       <c r="H13" s="0" t="inlineStr">
@@ -833,12 +833,12 @@
       </c>
       <c r="F14" s="0" t="inlineStr">
         <is>
-          <t>Blr</t>
+          <t>BLR</t>
         </is>
       </c>
       <c r="G14" s="0" t="inlineStr">
         <is>
-          <t>Del</t>
+          <t>DEL</t>
         </is>
       </c>
       <c r="H14" s="0" t="inlineStr">
@@ -875,12 +875,12 @@
       </c>
       <c r="F15" s="0" t="inlineStr">
         <is>
-          <t>Blr</t>
+          <t>BLR</t>
         </is>
       </c>
       <c r="G15" s="0" t="inlineStr">
         <is>
-          <t>Del</t>
+          <t>DEL</t>
         </is>
       </c>
       <c r="H15" s="0" t="inlineStr">
@@ -917,12 +917,12 @@
       </c>
       <c r="F16" s="0" t="inlineStr">
         <is>
-          <t>Blr</t>
+          <t>BLR</t>
         </is>
       </c>
       <c r="G16" s="0" t="inlineStr">
         <is>
-          <t>Del</t>
+          <t>DEL</t>
         </is>
       </c>
       <c r="H16" s="0" t="inlineStr">
@@ -959,12 +959,12 @@
       </c>
       <c r="F17" s="0" t="inlineStr">
         <is>
-          <t>Blr</t>
+          <t>BLR</t>
         </is>
       </c>
       <c r="G17" s="0" t="inlineStr">
         <is>
-          <t>Del</t>
+          <t>DEL</t>
         </is>
       </c>
       <c r="H17" s="0" t="inlineStr">
@@ -1001,12 +1001,12 @@
       </c>
       <c r="F18" s="0" t="inlineStr">
         <is>
-          <t>Del</t>
+          <t>DEL</t>
         </is>
       </c>
       <c r="G18" s="0" t="inlineStr">
         <is>
-          <t>Blr</t>
+          <t>BLR</t>
         </is>
       </c>
       <c r="H18" s="0" t="inlineStr">
@@ -1043,12 +1043,12 @@
       </c>
       <c r="F19" s="0" t="inlineStr">
         <is>
-          <t>Del</t>
+          <t>DEL</t>
         </is>
       </c>
       <c r="G19" s="0" t="inlineStr">
         <is>
-          <t>Blr</t>
+          <t>BLR</t>
         </is>
       </c>
       <c r="H19" s="0" t="inlineStr">
@@ -1085,12 +1085,12 @@
       </c>
       <c r="F20" s="0" t="inlineStr">
         <is>
-          <t>Del</t>
+          <t>DEL</t>
         </is>
       </c>
       <c r="G20" s="0" t="inlineStr">
         <is>
-          <t>Blr</t>
+          <t>BLR</t>
         </is>
       </c>
       <c r="H20" s="0" t="inlineStr">
@@ -1127,12 +1127,12 @@
       </c>
       <c r="F21" s="0" t="inlineStr">
         <is>
-          <t>Del</t>
+          <t>DEL</t>
         </is>
       </c>
       <c r="G21" s="0" t="inlineStr">
         <is>
-          <t>Blr</t>
+          <t>BLR</t>
         </is>
       </c>
       <c r="H21" s="0" t="inlineStr">
@@ -1169,12 +1169,12 @@
       </c>
       <c r="F22" s="0" t="inlineStr">
         <is>
-          <t>Del</t>
+          <t>DEL</t>
         </is>
       </c>
       <c r="G22" s="0" t="inlineStr">
         <is>
-          <t>Blr</t>
+          <t>BLR</t>
         </is>
       </c>
       <c r="H22" s="0" t="inlineStr">
@@ -1211,12 +1211,12 @@
       </c>
       <c r="F23" s="0" t="inlineStr">
         <is>
-          <t>Del</t>
+          <t>DEL</t>
         </is>
       </c>
       <c r="G23" s="0" t="inlineStr">
         <is>
-          <t>Blr</t>
+          <t>BLR</t>
         </is>
       </c>
       <c r="H23" s="0" t="inlineStr">
@@ -1253,12 +1253,12 @@
       </c>
       <c r="F24" s="0" t="inlineStr">
         <is>
-          <t>Del</t>
+          <t>DEL</t>
         </is>
       </c>
       <c r="G24" s="0" t="inlineStr">
         <is>
-          <t>Blr</t>
+          <t>BLR</t>
         </is>
       </c>
       <c r="H24" s="0" t="inlineStr">
@@ -1295,12 +1295,12 @@
       </c>
       <c r="F25" s="0" t="inlineStr">
         <is>
-          <t>Del</t>
+          <t>DEL</t>
         </is>
       </c>
       <c r="G25" s="0" t="inlineStr">
         <is>
-          <t>Blr</t>
+          <t>BLR</t>
         </is>
       </c>
       <c r="H25" s="0" t="inlineStr">
@@ -1337,12 +1337,12 @@
       </c>
       <c r="F26" s="0" t="inlineStr">
         <is>
-          <t>Del</t>
+          <t>DEL</t>
         </is>
       </c>
       <c r="G26" s="0" t="inlineStr">
         <is>
-          <t>Blr</t>
+          <t>BLR</t>
         </is>
       </c>
       <c r="H26" s="0" t="inlineStr">
@@ -1379,12 +1379,12 @@
       </c>
       <c r="F27" s="0" t="inlineStr">
         <is>
-          <t>Del</t>
+          <t>DEL</t>
         </is>
       </c>
       <c r="G27" s="0" t="inlineStr">
         <is>
-          <t>Blr</t>
+          <t>BLR</t>
         </is>
       </c>
       <c r="H27" s="0" t="inlineStr">
@@ -1421,12 +1421,12 @@
       </c>
       <c r="F28" s="0" t="inlineStr">
         <is>
-          <t>Del</t>
+          <t>DEL</t>
         </is>
       </c>
       <c r="G28" s="0" t="inlineStr">
         <is>
-          <t>Blr</t>
+          <t>BLR</t>
         </is>
       </c>
       <c r="H28" s="0" t="inlineStr">
@@ -1463,12 +1463,12 @@
       </c>
       <c r="F29" s="0" t="inlineStr">
         <is>
-          <t>Del</t>
+          <t>DEL</t>
         </is>
       </c>
       <c r="G29" s="0" t="inlineStr">
         <is>
-          <t>Blr</t>
+          <t>BLR</t>
         </is>
       </c>
       <c r="H29" s="0" t="inlineStr">
@@ -1505,12 +1505,12 @@
       </c>
       <c r="F30" s="0" t="inlineStr">
         <is>
-          <t>Del</t>
+          <t>DEL</t>
         </is>
       </c>
       <c r="G30" s="0" t="inlineStr">
         <is>
-          <t>Blr</t>
+          <t>BLR</t>
         </is>
       </c>
       <c r="H30" s="0" t="inlineStr">
@@ -1547,12 +1547,12 @@
       </c>
       <c r="F31" s="0" t="inlineStr">
         <is>
-          <t>Del</t>
+          <t>DEL</t>
         </is>
       </c>
       <c r="G31" s="0" t="inlineStr">
         <is>
-          <t>Blr</t>
+          <t>BLR</t>
         </is>
       </c>
       <c r="H31" s="0" t="inlineStr">
@@ -1589,12 +1589,12 @@
       </c>
       <c r="F32" s="0" t="inlineStr">
         <is>
-          <t>Del</t>
+          <t>DEL</t>
         </is>
       </c>
       <c r="G32" s="0" t="inlineStr">
         <is>
-          <t>Blr</t>
+          <t>BLR</t>
         </is>
       </c>
       <c r="H32" s="0" t="inlineStr">
@@ -1631,12 +1631,12 @@
       </c>
       <c r="F33" s="0" t="inlineStr">
         <is>
-          <t>Del</t>
+          <t>DEL</t>
         </is>
       </c>
       <c r="G33" s="0" t="inlineStr">
         <is>
-          <t>Blr</t>
+          <t>BLR</t>
         </is>
       </c>
       <c r="H33" s="0" t="inlineStr">
@@ -1673,12 +1673,12 @@
       </c>
       <c r="F34" s="0" t="inlineStr">
         <is>
-          <t>Blr</t>
+          <t>BLR</t>
         </is>
       </c>
       <c r="G34" s="0" t="inlineStr">
         <is>
-          <t>Del</t>
+          <t>DEL</t>
         </is>
       </c>
       <c r="H34" s="0" t="inlineStr">
@@ -1715,12 +1715,12 @@
       </c>
       <c r="F35" s="0" t="inlineStr">
         <is>
-          <t>Blr</t>
+          <t>BLR</t>
         </is>
       </c>
       <c r="G35" s="0" t="inlineStr">
         <is>
-          <t>Del</t>
+          <t>DEL</t>
         </is>
       </c>
       <c r="H35" s="0" t="inlineStr">
@@ -1730,1260 +1730,1260 @@
       </c>
     </row>
     <row r="36">
-      <c r="A36" t="inlineStr">
+      <c r="A36" s="0" t="inlineStr">
         <is>
           <t>f35</t>
         </is>
       </c>
-      <c r="B36" t="inlineStr">
+      <c r="B36" s="0" t="inlineStr">
         <is>
           <t>2019-10-23</t>
         </is>
       </c>
-      <c r="C36" t="inlineStr">
+      <c r="C36" s="0" t="inlineStr">
         <is>
           <t>Wed</t>
         </is>
       </c>
-      <c r="D36" t="inlineStr">
-        <is>
-          <t>Normal</t>
-        </is>
-      </c>
-      <c r="E36" t="inlineStr">
+      <c r="D36" s="0" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="E36" s="0" t="inlineStr">
         <is>
           <t>G8118</t>
         </is>
       </c>
-      <c r="F36" t="inlineStr">
-        <is>
-          <t>Blr</t>
-        </is>
-      </c>
-      <c r="G36" t="inlineStr">
-        <is>
-          <t>Del</t>
-        </is>
-      </c>
-      <c r="H36" t="inlineStr">
+      <c r="F36" s="0" t="inlineStr">
+        <is>
+          <t>BLR</t>
+        </is>
+      </c>
+      <c r="G36" s="0" t="inlineStr">
+        <is>
+          <t>DEL</t>
+        </is>
+      </c>
+      <c r="H36" s="0" t="inlineStr">
         <is>
           <t>2055</t>
         </is>
       </c>
     </row>
     <row r="37">
-      <c r="A37" t="inlineStr">
+      <c r="A37" s="0" t="inlineStr">
         <is>
           <t>f36</t>
         </is>
       </c>
-      <c r="B37" t="inlineStr">
+      <c r="B37" s="0" t="inlineStr">
         <is>
           <t>2019-10-23</t>
         </is>
       </c>
-      <c r="C37" t="inlineStr">
+      <c r="C37" s="0" t="inlineStr">
         <is>
           <t>Wed</t>
         </is>
       </c>
-      <c r="D37" t="inlineStr">
-        <is>
-          <t>Normal</t>
-        </is>
-      </c>
-      <c r="E37" t="inlineStr">
+      <c r="D37" s="0" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="E37" s="0" t="inlineStr">
         <is>
           <t>AI173</t>
         </is>
       </c>
-      <c r="F37" t="inlineStr">
-        <is>
-          <t>Blr</t>
-        </is>
-      </c>
-      <c r="G37" t="inlineStr">
-        <is>
-          <t>Del</t>
-        </is>
-      </c>
-      <c r="H37" t="inlineStr">
+      <c r="F37" s="0" t="inlineStr">
+        <is>
+          <t>BLR</t>
+        </is>
+      </c>
+      <c r="G37" s="0" t="inlineStr">
+        <is>
+          <t>DEL</t>
+        </is>
+      </c>
+      <c r="H37" s="0" t="inlineStr">
         <is>
           <t>2105</t>
         </is>
       </c>
     </row>
     <row r="38">
-      <c r="A38" t="inlineStr">
+      <c r="A38" s="0" t="inlineStr">
         <is>
           <t>f37</t>
         </is>
       </c>
-      <c r="B38" t="inlineStr">
+      <c r="B38" s="0" t="inlineStr">
         <is>
           <t>2019-10-24</t>
         </is>
       </c>
-      <c r="C38" t="inlineStr">
+      <c r="C38" s="0" t="inlineStr">
         <is>
           <t>Thu</t>
         </is>
       </c>
-      <c r="D38" t="inlineStr">
-        <is>
-          <t>Normal</t>
-        </is>
-      </c>
-      <c r="E38" t="inlineStr">
+      <c r="D38" s="0" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="E38" s="0" t="inlineStr">
         <is>
           <t>6E2484</t>
         </is>
       </c>
-      <c r="F38" t="inlineStr">
-        <is>
-          <t>Blr</t>
-        </is>
-      </c>
-      <c r="G38" t="inlineStr">
-        <is>
-          <t>Del</t>
-        </is>
-      </c>
-      <c r="H38" t="inlineStr">
+      <c r="F38" s="0" t="inlineStr">
+        <is>
+          <t>BLR</t>
+        </is>
+      </c>
+      <c r="G38" s="0" t="inlineStr">
+        <is>
+          <t>DEL</t>
+        </is>
+      </c>
+      <c r="H38" s="0" t="inlineStr">
         <is>
           <t>2330</t>
         </is>
       </c>
     </row>
     <row r="39">
-      <c r="A39" t="inlineStr">
+      <c r="A39" s="0" t="inlineStr">
         <is>
           <t>f38</t>
         </is>
       </c>
-      <c r="B39" t="inlineStr">
+      <c r="B39" s="0" t="inlineStr">
         <is>
           <t>2019-10-24</t>
         </is>
       </c>
-      <c r="C39" t="inlineStr">
+      <c r="C39" s="0" t="inlineStr">
         <is>
           <t>Thu</t>
         </is>
       </c>
-      <c r="D39" t="inlineStr">
-        <is>
-          <t>Normal</t>
-        </is>
-      </c>
-      <c r="E39" t="inlineStr">
+      <c r="D39" s="0" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="E39" s="0" t="inlineStr">
         <is>
           <t>SG8720</t>
         </is>
       </c>
-      <c r="F39" t="inlineStr">
-        <is>
-          <t>Blr</t>
-        </is>
-      </c>
-      <c r="G39" t="inlineStr">
-        <is>
-          <t>Del</t>
-        </is>
-      </c>
-      <c r="H39" t="inlineStr">
+      <c r="F39" s="0" t="inlineStr">
+        <is>
+          <t>BLR</t>
+        </is>
+      </c>
+      <c r="G39" s="0" t="inlineStr">
+        <is>
+          <t>DEL</t>
+        </is>
+      </c>
+      <c r="H39" s="0" t="inlineStr">
         <is>
           <t>2200</t>
         </is>
       </c>
     </row>
     <row r="40">
-      <c r="A40" t="inlineStr">
+      <c r="A40" s="0" t="inlineStr">
         <is>
           <t>f39</t>
         </is>
       </c>
-      <c r="B40" t="inlineStr">
+      <c r="B40" s="0" t="inlineStr">
         <is>
           <t>2019-10-24</t>
         </is>
       </c>
-      <c r="C40" t="inlineStr">
+      <c r="C40" s="0" t="inlineStr">
         <is>
           <t>Thu</t>
         </is>
       </c>
-      <c r="D40" t="inlineStr">
-        <is>
-          <t>Normal</t>
-        </is>
-      </c>
-      <c r="E40" t="inlineStr">
+      <c r="D40" s="0" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="E40" s="0" t="inlineStr">
         <is>
           <t>G8118</t>
         </is>
       </c>
-      <c r="F40" t="inlineStr">
-        <is>
-          <t>Blr</t>
-        </is>
-      </c>
-      <c r="G40" t="inlineStr">
-        <is>
-          <t>Del</t>
-        </is>
-      </c>
-      <c r="H40" t="inlineStr">
+      <c r="F40" s="0" t="inlineStr">
+        <is>
+          <t>BLR</t>
+        </is>
+      </c>
+      <c r="G40" s="0" t="inlineStr">
+        <is>
+          <t>DEL</t>
+        </is>
+      </c>
+      <c r="H40" s="0" t="inlineStr">
         <is>
           <t>2055</t>
         </is>
       </c>
     </row>
     <row r="41">
-      <c r="A41" t="inlineStr">
+      <c r="A41" s="0" t="inlineStr">
         <is>
           <t>f40</t>
         </is>
       </c>
-      <c r="B41" t="inlineStr">
+      <c r="B41" s="0" t="inlineStr">
         <is>
           <t>2019-10-24</t>
         </is>
       </c>
-      <c r="C41" t="inlineStr">
+      <c r="C41" s="0" t="inlineStr">
         <is>
           <t>Thu</t>
         </is>
       </c>
-      <c r="D41" t="inlineStr">
-        <is>
-          <t>Normal</t>
-        </is>
-      </c>
-      <c r="E41" t="inlineStr">
+      <c r="D41" s="0" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="E41" s="0" t="inlineStr">
         <is>
           <t>AI173</t>
         </is>
       </c>
-      <c r="F41" t="inlineStr">
-        <is>
-          <t>Blr</t>
-        </is>
-      </c>
-      <c r="G41" t="inlineStr">
-        <is>
-          <t>Del</t>
-        </is>
-      </c>
-      <c r="H41" t="inlineStr">
+      <c r="F41" s="0" t="inlineStr">
+        <is>
+          <t>BLR</t>
+        </is>
+      </c>
+      <c r="G41" s="0" t="inlineStr">
+        <is>
+          <t>DEL</t>
+        </is>
+      </c>
+      <c r="H41" s="0" t="inlineStr">
         <is>
           <t>2105</t>
         </is>
       </c>
     </row>
     <row r="42">
-      <c r="A42" t="inlineStr">
+      <c r="A42" s="0" t="inlineStr">
         <is>
           <t>f41</t>
         </is>
       </c>
-      <c r="B42" t="inlineStr">
+      <c r="B42" s="0" t="inlineStr">
         <is>
           <t>2019-11-06</t>
         </is>
       </c>
-      <c r="C42" t="inlineStr">
+      <c r="C42" s="0" t="inlineStr">
         <is>
           <t>Wed</t>
         </is>
       </c>
-      <c r="D42" t="inlineStr">
-        <is>
-          <t>Normal</t>
-        </is>
-      </c>
-      <c r="E42" t="inlineStr">
+      <c r="D42" s="0" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="E42" s="0" t="inlineStr">
         <is>
           <t>6E2484</t>
         </is>
       </c>
-      <c r="F42" t="inlineStr">
-        <is>
-          <t>Blr</t>
-        </is>
-      </c>
-      <c r="G42" t="inlineStr">
-        <is>
-          <t>Del</t>
-        </is>
-      </c>
-      <c r="H42" t="inlineStr">
+      <c r="F42" s="0" t="inlineStr">
+        <is>
+          <t>BLR</t>
+        </is>
+      </c>
+      <c r="G42" s="0" t="inlineStr">
+        <is>
+          <t>DEL</t>
+        </is>
+      </c>
+      <c r="H42" s="0" t="inlineStr">
         <is>
           <t>2330</t>
         </is>
       </c>
     </row>
     <row r="43">
-      <c r="A43" t="inlineStr">
+      <c r="A43" s="0" t="inlineStr">
         <is>
           <t>f42</t>
         </is>
       </c>
-      <c r="B43" t="inlineStr">
+      <c r="B43" s="0" t="inlineStr">
         <is>
           <t>2019-11-06</t>
         </is>
       </c>
-      <c r="C43" t="inlineStr">
+      <c r="C43" s="0" t="inlineStr">
         <is>
           <t>Wed</t>
         </is>
       </c>
-      <c r="D43" t="inlineStr">
-        <is>
-          <t>Normal</t>
-        </is>
-      </c>
-      <c r="E43" t="inlineStr">
+      <c r="D43" s="0" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="E43" s="0" t="inlineStr">
         <is>
           <t>SG8720</t>
         </is>
       </c>
-      <c r="F43" t="inlineStr">
-        <is>
-          <t>Blr</t>
-        </is>
-      </c>
-      <c r="G43" t="inlineStr">
-        <is>
-          <t>Del</t>
-        </is>
-      </c>
-      <c r="H43" t="inlineStr">
+      <c r="F43" s="0" t="inlineStr">
+        <is>
+          <t>BLR</t>
+        </is>
+      </c>
+      <c r="G43" s="0" t="inlineStr">
+        <is>
+          <t>DEL</t>
+        </is>
+      </c>
+      <c r="H43" s="0" t="inlineStr">
         <is>
           <t>2200</t>
         </is>
       </c>
     </row>
     <row r="44">
-      <c r="A44" t="inlineStr">
+      <c r="A44" s="0" t="inlineStr">
         <is>
           <t>f43</t>
         </is>
       </c>
-      <c r="B44" t="inlineStr">
+      <c r="B44" s="0" t="inlineStr">
         <is>
           <t>2019-11-06</t>
         </is>
       </c>
-      <c r="C44" t="inlineStr">
+      <c r="C44" s="0" t="inlineStr">
         <is>
           <t>Wed</t>
         </is>
       </c>
-      <c r="D44" t="inlineStr">
-        <is>
-          <t>Normal</t>
-        </is>
-      </c>
-      <c r="E44" t="inlineStr">
+      <c r="D44" s="0" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="E44" s="0" t="inlineStr">
         <is>
           <t>G8120</t>
         </is>
       </c>
-      <c r="F44" t="inlineStr">
-        <is>
-          <t>Blr</t>
-        </is>
-      </c>
-      <c r="G44" t="inlineStr">
-        <is>
-          <t>Del</t>
-        </is>
-      </c>
-      <c r="H44" t="inlineStr">
+      <c r="F44" s="0" t="inlineStr">
+        <is>
+          <t>BLR</t>
+        </is>
+      </c>
+      <c r="G44" s="0" t="inlineStr">
+        <is>
+          <t>DEL</t>
+        </is>
+      </c>
+      <c r="H44" s="0" t="inlineStr">
         <is>
           <t>1140</t>
         </is>
       </c>
     </row>
     <row r="45">
-      <c r="A45" t="inlineStr">
+      <c r="A45" s="0" t="inlineStr">
         <is>
           <t>f44</t>
         </is>
       </c>
-      <c r="B45" t="inlineStr">
+      <c r="B45" s="0" t="inlineStr">
         <is>
           <t>2019-11-06</t>
         </is>
       </c>
-      <c r="C45" t="inlineStr">
+      <c r="C45" s="0" t="inlineStr">
         <is>
           <t>Wed</t>
         </is>
       </c>
-      <c r="D45" t="inlineStr">
-        <is>
-          <t>Normal</t>
-        </is>
-      </c>
-      <c r="E45" t="inlineStr">
+      <c r="D45" s="0" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="E45" s="0" t="inlineStr">
         <is>
           <t>AI173</t>
         </is>
       </c>
-      <c r="F45" t="inlineStr">
-        <is>
-          <t>Blr</t>
-        </is>
-      </c>
-      <c r="G45" t="inlineStr">
-        <is>
-          <t>Del</t>
-        </is>
-      </c>
-      <c r="H45" t="inlineStr">
+      <c r="F45" s="0" t="inlineStr">
+        <is>
+          <t>BLR</t>
+        </is>
+      </c>
+      <c r="G45" s="0" t="inlineStr">
+        <is>
+          <t>DEL</t>
+        </is>
+      </c>
+      <c r="H45" s="0" t="inlineStr">
         <is>
           <t>2110</t>
         </is>
       </c>
     </row>
     <row r="46">
-      <c r="A46" t="inlineStr">
+      <c r="A46" s="0" t="inlineStr">
         <is>
           <t>f45</t>
         </is>
       </c>
-      <c r="B46" t="inlineStr">
+      <c r="B46" s="0" t="inlineStr">
         <is>
           <t>2019-09-07</t>
         </is>
       </c>
-      <c r="C46" t="inlineStr">
+      <c r="C46" s="0" t="inlineStr">
         <is>
           <t>Thu</t>
         </is>
       </c>
-      <c r="D46" t="inlineStr">
-        <is>
-          <t>Normal</t>
-        </is>
-      </c>
-      <c r="E46" t="inlineStr">
+      <c r="D46" s="0" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="E46" s="0" t="inlineStr">
         <is>
           <t>6E2484</t>
         </is>
       </c>
-      <c r="F46" t="inlineStr">
-        <is>
-          <t>Blr</t>
-        </is>
-      </c>
-      <c r="G46" t="inlineStr">
-        <is>
-          <t>Del</t>
-        </is>
-      </c>
-      <c r="H46" t="inlineStr">
+      <c r="F46" s="0" t="inlineStr">
+        <is>
+          <t>BLR</t>
+        </is>
+      </c>
+      <c r="G46" s="0" t="inlineStr">
+        <is>
+          <t>DEL</t>
+        </is>
+      </c>
+      <c r="H46" s="0" t="inlineStr">
         <is>
           <t>2330</t>
         </is>
       </c>
     </row>
     <row r="47">
-      <c r="A47" t="inlineStr">
+      <c r="A47" s="0" t="inlineStr">
         <is>
           <t>f46</t>
         </is>
       </c>
-      <c r="B47" t="inlineStr">
+      <c r="B47" s="0" t="inlineStr">
         <is>
           <t>2019-09-07</t>
         </is>
       </c>
-      <c r="C47" t="inlineStr">
+      <c r="C47" s="0" t="inlineStr">
         <is>
           <t>Thu</t>
         </is>
       </c>
-      <c r="D47" t="inlineStr">
-        <is>
-          <t>Normal</t>
-        </is>
-      </c>
-      <c r="E47" t="inlineStr">
+      <c r="D47" s="0" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="E47" s="0" t="inlineStr">
         <is>
           <t>SG8720</t>
         </is>
       </c>
-      <c r="F47" t="inlineStr">
-        <is>
-          <t>Blr</t>
-        </is>
-      </c>
-      <c r="G47" t="inlineStr">
-        <is>
-          <t>Del</t>
-        </is>
-      </c>
-      <c r="H47" t="inlineStr">
+      <c r="F47" s="0" t="inlineStr">
+        <is>
+          <t>BLR</t>
+        </is>
+      </c>
+      <c r="G47" s="0" t="inlineStr">
+        <is>
+          <t>DEL</t>
+        </is>
+      </c>
+      <c r="H47" s="0" t="inlineStr">
         <is>
           <t>2200</t>
         </is>
       </c>
     </row>
     <row r="48">
-      <c r="A48" t="inlineStr">
+      <c r="A48" s="0" t="inlineStr">
         <is>
           <t>f47</t>
         </is>
       </c>
-      <c r="B48" t="inlineStr">
+      <c r="B48" s="0" t="inlineStr">
         <is>
           <t>2019-09-07</t>
         </is>
       </c>
-      <c r="C48" t="inlineStr">
+      <c r="C48" s="0" t="inlineStr">
         <is>
           <t>Thu</t>
         </is>
       </c>
-      <c r="D48" t="inlineStr">
-        <is>
-          <t>Normal</t>
-        </is>
-      </c>
-      <c r="E48" t="inlineStr">
+      <c r="D48" s="0" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="E48" s="0" t="inlineStr">
         <is>
           <t>G8120</t>
         </is>
       </c>
-      <c r="F48" t="inlineStr">
-        <is>
-          <t>Blr</t>
-        </is>
-      </c>
-      <c r="G48" t="inlineStr">
-        <is>
-          <t>Del</t>
-        </is>
-      </c>
-      <c r="H48" t="inlineStr">
+      <c r="F48" s="0" t="inlineStr">
+        <is>
+          <t>BLR</t>
+        </is>
+      </c>
+      <c r="G48" s="0" t="inlineStr">
+        <is>
+          <t>DEL</t>
+        </is>
+      </c>
+      <c r="H48" s="0" t="inlineStr">
         <is>
           <t>1140</t>
         </is>
       </c>
     </row>
     <row r="49">
-      <c r="A49" t="inlineStr">
+      <c r="A49" s="0" t="inlineStr">
         <is>
           <t>f48</t>
         </is>
       </c>
-      <c r="B49" t="inlineStr">
+      <c r="B49" s="0" t="inlineStr">
         <is>
           <t>2019-09-07</t>
         </is>
       </c>
-      <c r="C49" t="inlineStr">
+      <c r="C49" s="0" t="inlineStr">
         <is>
           <t>Thu</t>
         </is>
       </c>
-      <c r="D49" t="inlineStr">
-        <is>
-          <t>Normal</t>
-        </is>
-      </c>
-      <c r="E49" t="inlineStr">
+      <c r="D49" s="0" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="E49" s="0" t="inlineStr">
         <is>
           <t>AI173</t>
         </is>
       </c>
-      <c r="F49" t="inlineStr">
-        <is>
-          <t>Blr</t>
-        </is>
-      </c>
-      <c r="G49" t="inlineStr">
-        <is>
-          <t>Del</t>
-        </is>
-      </c>
-      <c r="H49" t="inlineStr">
+      <c r="F49" s="0" t="inlineStr">
+        <is>
+          <t>BLR</t>
+        </is>
+      </c>
+      <c r="G49" s="0" t="inlineStr">
+        <is>
+          <t>DEL</t>
+        </is>
+      </c>
+      <c r="H49" s="0" t="inlineStr">
         <is>
           <t>2110</t>
         </is>
       </c>
     </row>
     <row r="50">
-      <c r="A50" t="inlineStr">
+      <c r="A50" s="0" t="inlineStr">
         <is>
           <t>f49</t>
         </is>
       </c>
-      <c r="B50" t="inlineStr">
+      <c r="B50" s="0" t="inlineStr">
         <is>
           <t>2019-10-23</t>
         </is>
       </c>
-      <c r="C50" t="inlineStr">
+      <c r="C50" s="0" t="inlineStr">
         <is>
           <t>Wed</t>
         </is>
       </c>
-      <c r="D50" t="inlineStr">
-        <is>
-          <t>Normal</t>
-        </is>
-      </c>
-      <c r="E50" t="inlineStr">
+      <c r="D50" s="0" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="E50" s="0" t="inlineStr">
         <is>
           <t>6E2458</t>
         </is>
       </c>
-      <c r="F50" t="inlineStr">
-        <is>
-          <t>Del</t>
-        </is>
-      </c>
-      <c r="G50" t="inlineStr">
-        <is>
-          <t>Blr</t>
-        </is>
-      </c>
-      <c r="H50" t="inlineStr">
+      <c r="F50" s="0" t="inlineStr">
+        <is>
+          <t>DEL</t>
+        </is>
+      </c>
+      <c r="G50" s="0" t="inlineStr">
+        <is>
+          <t>BLR</t>
+        </is>
+      </c>
+      <c r="H50" s="0" t="inlineStr">
         <is>
           <t>0625</t>
         </is>
       </c>
     </row>
     <row r="51">
-      <c r="A51" t="inlineStr">
+      <c r="A51" s="0" t="inlineStr">
         <is>
           <t>f50</t>
         </is>
       </c>
-      <c r="B51" t="inlineStr">
+      <c r="B51" s="0" t="inlineStr">
         <is>
           <t>2019-10-23</t>
         </is>
       </c>
-      <c r="C51" t="inlineStr">
+      <c r="C51" s="0" t="inlineStr">
         <is>
           <t>Wed</t>
         </is>
       </c>
-      <c r="D51" t="inlineStr">
-        <is>
-          <t>Normal</t>
-        </is>
-      </c>
-      <c r="E51" t="inlineStr">
+      <c r="D51" s="0" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="E51" s="0" t="inlineStr">
         <is>
           <t>SG191</t>
         </is>
       </c>
-      <c r="F51" t="inlineStr">
-        <is>
-          <t>Del</t>
-        </is>
-      </c>
-      <c r="G51" t="inlineStr">
-        <is>
-          <t>Blr</t>
-        </is>
-      </c>
-      <c r="H51" t="inlineStr">
+      <c r="F51" s="0" t="inlineStr">
+        <is>
+          <t>DEL</t>
+        </is>
+      </c>
+      <c r="G51" s="0" t="inlineStr">
+        <is>
+          <t>BLR</t>
+        </is>
+      </c>
+      <c r="H51" s="0" t="inlineStr">
         <is>
           <t>0610</t>
         </is>
       </c>
     </row>
     <row r="52">
-      <c r="A52" t="inlineStr">
+      <c r="A52" s="0" t="inlineStr">
         <is>
           <t>f51</t>
         </is>
       </c>
-      <c r="B52" t="inlineStr">
+      <c r="B52" s="0" t="inlineStr">
         <is>
           <t>2019-10-23</t>
         </is>
       </c>
-      <c r="C52" t="inlineStr">
+      <c r="C52" s="0" t="inlineStr">
         <is>
           <t>Wed</t>
         </is>
       </c>
-      <c r="D52" t="inlineStr">
-        <is>
-          <t>Normal</t>
-        </is>
-      </c>
-      <c r="E52" t="inlineStr">
+      <c r="D52" s="0" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="E52" s="0" t="inlineStr">
         <is>
           <t>G8113</t>
         </is>
       </c>
-      <c r="F52" t="inlineStr">
-        <is>
-          <t>Del</t>
-        </is>
-      </c>
-      <c r="G52" t="inlineStr">
-        <is>
-          <t>Blr</t>
-        </is>
-      </c>
-      <c r="H52" t="inlineStr">
+      <c r="F52" s="0" t="inlineStr">
+        <is>
+          <t>DEL</t>
+        </is>
+      </c>
+      <c r="G52" s="0" t="inlineStr">
+        <is>
+          <t>BLR</t>
+        </is>
+      </c>
+      <c r="H52" s="0" t="inlineStr">
         <is>
           <t>0550</t>
         </is>
       </c>
     </row>
     <row r="53">
-      <c r="A53" t="inlineStr">
+      <c r="A53" s="0" t="inlineStr">
         <is>
           <t>f52</t>
         </is>
       </c>
-      <c r="B53" t="inlineStr">
+      <c r="B53" s="0" t="inlineStr">
         <is>
           <t>2019-10-23</t>
         </is>
       </c>
-      <c r="C53" t="inlineStr">
+      <c r="C53" s="0" t="inlineStr">
         <is>
           <t>Wed</t>
         </is>
       </c>
-      <c r="D53" t="inlineStr">
-        <is>
-          <t>Normal</t>
-        </is>
-      </c>
-      <c r="E53" t="inlineStr">
+      <c r="D53" s="0" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="E53" s="0" t="inlineStr">
         <is>
           <t>AI803</t>
         </is>
       </c>
-      <c r="F53" t="inlineStr">
-        <is>
-          <t>Del</t>
-        </is>
-      </c>
-      <c r="G53" t="inlineStr">
-        <is>
-          <t>Blr</t>
-        </is>
-      </c>
-      <c r="H53" t="inlineStr">
+      <c r="F53" s="0" t="inlineStr">
+        <is>
+          <t>DEL</t>
+        </is>
+      </c>
+      <c r="G53" s="0" t="inlineStr">
+        <is>
+          <t>BLR</t>
+        </is>
+      </c>
+      <c r="H53" s="0" t="inlineStr">
         <is>
           <t>0610</t>
         </is>
       </c>
     </row>
     <row r="54">
-      <c r="A54" t="inlineStr">
+      <c r="A54" s="0" t="inlineStr">
         <is>
           <t>f53</t>
         </is>
       </c>
-      <c r="B54" t="inlineStr">
+      <c r="B54" s="0" t="inlineStr">
         <is>
           <t>2019-10-24</t>
         </is>
       </c>
-      <c r="C54" t="inlineStr">
+      <c r="C54" s="0" t="inlineStr">
         <is>
           <t>Thu</t>
         </is>
       </c>
-      <c r="D54" t="inlineStr">
-        <is>
-          <t>Normal</t>
-        </is>
-      </c>
-      <c r="E54" t="inlineStr">
+      <c r="D54" s="0" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="E54" s="0" t="inlineStr">
         <is>
           <t>6E5031</t>
         </is>
       </c>
-      <c r="F54" t="inlineStr">
-        <is>
-          <t>Del</t>
-        </is>
-      </c>
-      <c r="G54" t="inlineStr">
-        <is>
-          <t>Blr</t>
-        </is>
-      </c>
-      <c r="H54" t="inlineStr">
+      <c r="F54" s="0" t="inlineStr">
+        <is>
+          <t>DEL</t>
+        </is>
+      </c>
+      <c r="G54" s="0" t="inlineStr">
+        <is>
+          <t>BLR</t>
+        </is>
+      </c>
+      <c r="H54" s="0" t="inlineStr">
         <is>
           <t>0505</t>
         </is>
       </c>
     </row>
     <row r="55">
-      <c r="A55" t="inlineStr">
+      <c r="A55" s="0" t="inlineStr">
         <is>
           <t>f54</t>
         </is>
       </c>
-      <c r="B55" t="inlineStr">
+      <c r="B55" s="0" t="inlineStr">
         <is>
           <t>2019-10-24</t>
         </is>
       </c>
-      <c r="C55" t="inlineStr">
+      <c r="C55" s="0" t="inlineStr">
         <is>
           <t>Thu</t>
         </is>
       </c>
-      <c r="D55" t="inlineStr">
-        <is>
-          <t>Normal</t>
-        </is>
-      </c>
-      <c r="E55" t="inlineStr">
+      <c r="D55" s="0" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="E55" s="0" t="inlineStr">
         <is>
           <t>SG191</t>
         </is>
       </c>
-      <c r="F55" t="inlineStr">
-        <is>
-          <t>Del</t>
-        </is>
-      </c>
-      <c r="G55" t="inlineStr">
-        <is>
-          <t>Blr</t>
-        </is>
-      </c>
-      <c r="H55" t="inlineStr">
+      <c r="F55" s="0" t="inlineStr">
+        <is>
+          <t>DEL</t>
+        </is>
+      </c>
+      <c r="G55" s="0" t="inlineStr">
+        <is>
+          <t>BLR</t>
+        </is>
+      </c>
+      <c r="H55" s="0" t="inlineStr">
         <is>
           <t>0610</t>
         </is>
       </c>
     </row>
     <row r="56">
-      <c r="A56" t="inlineStr">
+      <c r="A56" s="0" t="inlineStr">
         <is>
           <t>f55</t>
         </is>
       </c>
-      <c r="B56" t="inlineStr">
+      <c r="B56" s="0" t="inlineStr">
         <is>
           <t>2019-10-24</t>
         </is>
       </c>
-      <c r="C56" t="inlineStr">
+      <c r="C56" s="0" t="inlineStr">
         <is>
           <t>Thu</t>
         </is>
       </c>
-      <c r="D56" t="inlineStr">
-        <is>
-          <t>Normal</t>
-        </is>
-      </c>
-      <c r="E56" t="inlineStr">
+      <c r="D56" s="0" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="E56" s="0" t="inlineStr">
         <is>
           <t>G8113</t>
         </is>
       </c>
-      <c r="F56" t="inlineStr">
-        <is>
-          <t>Del</t>
-        </is>
-      </c>
-      <c r="G56" t="inlineStr">
-        <is>
-          <t>Blr</t>
-        </is>
-      </c>
-      <c r="H56" t="inlineStr">
+      <c r="F56" s="0" t="inlineStr">
+        <is>
+          <t>DEL</t>
+        </is>
+      </c>
+      <c r="G56" s="0" t="inlineStr">
+        <is>
+          <t>BLR</t>
+        </is>
+      </c>
+      <c r="H56" s="0" t="inlineStr">
         <is>
           <t>0550</t>
         </is>
       </c>
     </row>
     <row r="57">
-      <c r="A57" t="inlineStr">
+      <c r="A57" s="0" t="inlineStr">
         <is>
           <t>f56</t>
         </is>
       </c>
-      <c r="B57" t="inlineStr">
+      <c r="B57" s="0" t="inlineStr">
         <is>
           <t>2019-10-24</t>
         </is>
       </c>
-      <c r="C57" t="inlineStr">
+      <c r="C57" s="0" t="inlineStr">
         <is>
           <t>Thu</t>
         </is>
       </c>
-      <c r="D57" t="inlineStr">
-        <is>
-          <t>Normal</t>
-        </is>
-      </c>
-      <c r="E57" t="inlineStr">
+      <c r="D57" s="0" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="E57" s="0" t="inlineStr">
         <is>
           <t>AI803</t>
         </is>
       </c>
-      <c r="F57" t="inlineStr">
-        <is>
-          <t>Del</t>
-        </is>
-      </c>
-      <c r="G57" t="inlineStr">
-        <is>
-          <t>Blr</t>
-        </is>
-      </c>
-      <c r="H57" t="inlineStr">
+      <c r="F57" s="0" t="inlineStr">
+        <is>
+          <t>DEL</t>
+        </is>
+      </c>
+      <c r="G57" s="0" t="inlineStr">
+        <is>
+          <t>BLR</t>
+        </is>
+      </c>
+      <c r="H57" s="0" t="inlineStr">
         <is>
           <t>0610</t>
         </is>
       </c>
     </row>
     <row r="58">
-      <c r="A58" t="inlineStr">
+      <c r="A58" s="0" t="inlineStr">
         <is>
           <t>f57</t>
         </is>
       </c>
-      <c r="B58" t="inlineStr">
+      <c r="B58" s="0" t="inlineStr">
         <is>
           <t>2019-11-06</t>
         </is>
       </c>
-      <c r="C58" t="inlineStr">
+      <c r="C58" s="0" t="inlineStr">
         <is>
           <t>Wed</t>
         </is>
       </c>
-      <c r="D58" t="inlineStr">
-        <is>
-          <t>Normal</t>
-        </is>
-      </c>
-      <c r="E58" t="inlineStr">
+      <c r="D58" s="0" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="E58" s="0" t="inlineStr">
         <is>
           <t>6E2134</t>
         </is>
       </c>
-      <c r="F58" t="inlineStr">
-        <is>
-          <t>Del</t>
-        </is>
-      </c>
-      <c r="G58" t="inlineStr">
-        <is>
-          <t>Blr</t>
-        </is>
-      </c>
-      <c r="H58" t="inlineStr">
+      <c r="F58" s="0" t="inlineStr">
+        <is>
+          <t>DEL</t>
+        </is>
+      </c>
+      <c r="G58" s="0" t="inlineStr">
+        <is>
+          <t>BLR</t>
+        </is>
+      </c>
+      <c r="H58" s="0" t="inlineStr">
         <is>
           <t>0305</t>
         </is>
       </c>
     </row>
     <row r="59">
-      <c r="A59" t="inlineStr">
+      <c r="A59" s="0" t="inlineStr">
         <is>
           <t>f58</t>
         </is>
       </c>
-      <c r="B59" t="inlineStr">
+      <c r="B59" s="0" t="inlineStr">
         <is>
           <t>2019-11-06</t>
         </is>
       </c>
-      <c r="C59" t="inlineStr">
+      <c r="C59" s="0" t="inlineStr">
         <is>
           <t>Wed</t>
         </is>
       </c>
-      <c r="D59" t="inlineStr">
-        <is>
-          <t>Normal</t>
-        </is>
-      </c>
-      <c r="E59" t="inlineStr">
+      <c r="D59" s="0" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="E59" s="0" t="inlineStr">
         <is>
           <t>SG191</t>
         </is>
       </c>
-      <c r="F59" t="inlineStr">
-        <is>
-          <t>Del</t>
-        </is>
-      </c>
-      <c r="G59" t="inlineStr">
-        <is>
-          <t>Blr</t>
-        </is>
-      </c>
-      <c r="H59" t="inlineStr">
+      <c r="F59" s="0" t="inlineStr">
+        <is>
+          <t>DEL</t>
+        </is>
+      </c>
+      <c r="G59" s="0" t="inlineStr">
+        <is>
+          <t>BLR</t>
+        </is>
+      </c>
+      <c r="H59" s="0" t="inlineStr">
         <is>
           <t>0620</t>
         </is>
       </c>
     </row>
     <row r="60">
-      <c r="A60" t="inlineStr">
+      <c r="A60" s="0" t="inlineStr">
         <is>
           <t>f59</t>
         </is>
       </c>
-      <c r="B60" t="inlineStr">
+      <c r="B60" s="0" t="inlineStr">
         <is>
           <t>2019-11-06</t>
         </is>
       </c>
-      <c r="C60" t="inlineStr">
+      <c r="C60" s="0" t="inlineStr">
         <is>
           <t>Wed</t>
         </is>
       </c>
-      <c r="D60" t="inlineStr">
-        <is>
-          <t>Normal</t>
-        </is>
-      </c>
-      <c r="E60" t="inlineStr">
+      <c r="D60" s="0" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="E60" s="0" t="inlineStr">
         <is>
           <t>G8113</t>
         </is>
       </c>
-      <c r="F60" t="inlineStr">
-        <is>
-          <t>Del</t>
-        </is>
-      </c>
-      <c r="G60" t="inlineStr">
-        <is>
-          <t>Blr</t>
-        </is>
-      </c>
-      <c r="H60" t="inlineStr">
+      <c r="F60" s="0" t="inlineStr">
+        <is>
+          <t>DEL</t>
+        </is>
+      </c>
+      <c r="G60" s="0" t="inlineStr">
+        <is>
+          <t>BLR</t>
+        </is>
+      </c>
+      <c r="H60" s="0" t="inlineStr">
         <is>
           <t>0505</t>
         </is>
       </c>
     </row>
     <row r="61">
-      <c r="A61" t="inlineStr">
+      <c r="A61" s="0" t="inlineStr">
         <is>
           <t>f60</t>
         </is>
       </c>
-      <c r="B61" t="inlineStr">
+      <c r="B61" s="0" t="inlineStr">
         <is>
           <t>2019-11-06</t>
         </is>
       </c>
-      <c r="C61" t="inlineStr">
+      <c r="C61" s="0" t="inlineStr">
         <is>
           <t>Wed</t>
         </is>
       </c>
-      <c r="D61" t="inlineStr">
-        <is>
-          <t>Normal</t>
-        </is>
-      </c>
-      <c r="E61" t="inlineStr">
+      <c r="D61" s="0" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="E61" s="0" t="inlineStr">
         <is>
           <t>AI803</t>
         </is>
       </c>
-      <c r="F61" t="inlineStr">
-        <is>
-          <t>Del</t>
-        </is>
-      </c>
-      <c r="G61" t="inlineStr">
-        <is>
-          <t>Blr</t>
-        </is>
-      </c>
-      <c r="H61" t="inlineStr">
+      <c r="F61" s="0" t="inlineStr">
+        <is>
+          <t>DEL</t>
+        </is>
+      </c>
+      <c r="G61" s="0" t="inlineStr">
+        <is>
+          <t>BLR</t>
+        </is>
+      </c>
+      <c r="H61" s="0" t="inlineStr">
         <is>
           <t>0610</t>
         </is>
       </c>
     </row>
     <row r="62">
-      <c r="A62" t="inlineStr">
+      <c r="A62" s="0" t="inlineStr">
         <is>
           <t>f61</t>
         </is>
       </c>
-      <c r="B62" t="inlineStr">
+      <c r="B62" s="0" t="inlineStr">
         <is>
           <t>2019-11-07</t>
         </is>
       </c>
-      <c r="C62" t="inlineStr">
+      <c r="C62" s="0" t="inlineStr">
         <is>
           <t>Thu</t>
         </is>
       </c>
-      <c r="D62" t="inlineStr">
-        <is>
-          <t>Normal</t>
-        </is>
-      </c>
-      <c r="E62" t="inlineStr">
+      <c r="D62" s="0" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="E62" s="0" t="inlineStr">
         <is>
           <t>6E5015</t>
         </is>
       </c>
-      <c r="F62" t="inlineStr">
-        <is>
-          <t>Del</t>
-        </is>
-      </c>
-      <c r="G62" t="inlineStr">
-        <is>
-          <t>Blr</t>
-        </is>
-      </c>
-      <c r="H62" t="inlineStr">
+      <c r="F62" s="0" t="inlineStr">
+        <is>
+          <t>DEL</t>
+        </is>
+      </c>
+      <c r="G62" s="0" t="inlineStr">
+        <is>
+          <t>BLR</t>
+        </is>
+      </c>
+      <c r="H62" s="0" t="inlineStr">
         <is>
           <t>0755</t>
         </is>
       </c>
     </row>
     <row r="63">
-      <c r="A63" t="inlineStr">
+      <c r="A63" s="0" t="inlineStr">
         <is>
           <t>f62</t>
         </is>
       </c>
-      <c r="B63" t="inlineStr">
+      <c r="B63" s="0" t="inlineStr">
         <is>
           <t>2019-11-07</t>
         </is>
       </c>
-      <c r="C63" t="inlineStr">
+      <c r="C63" s="0" t="inlineStr">
         <is>
           <t>Thu</t>
         </is>
       </c>
-      <c r="D63" t="inlineStr">
-        <is>
-          <t>Normal</t>
-        </is>
-      </c>
-      <c r="E63" t="inlineStr">
+      <c r="D63" s="0" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="E63" s="0" t="inlineStr">
         <is>
           <t>SG191</t>
         </is>
       </c>
-      <c r="F63" t="inlineStr">
-        <is>
-          <t>Del</t>
-        </is>
-      </c>
-      <c r="G63" t="inlineStr">
-        <is>
-          <t>Blr</t>
-        </is>
-      </c>
-      <c r="H63" t="inlineStr">
+      <c r="F63" s="0" t="inlineStr">
+        <is>
+          <t>DEL</t>
+        </is>
+      </c>
+      <c r="G63" s="0" t="inlineStr">
+        <is>
+          <t>BLR</t>
+        </is>
+      </c>
+      <c r="H63" s="0" t="inlineStr">
         <is>
           <t>0620</t>
         </is>
       </c>
     </row>
     <row r="64">
-      <c r="A64" t="inlineStr">
+      <c r="A64" s="0" t="inlineStr">
         <is>
           <t>f63</t>
         </is>
       </c>
-      <c r="B64" t="inlineStr">
+      <c r="B64" s="0" t="inlineStr">
         <is>
           <t>2019-11-07</t>
         </is>
       </c>
-      <c r="C64" t="inlineStr">
+      <c r="C64" s="0" t="inlineStr">
         <is>
           <t>Thu</t>
         </is>
       </c>
-      <c r="D64" t="inlineStr">
-        <is>
-          <t>Normal</t>
-        </is>
-      </c>
-      <c r="E64" t="inlineStr">
+      <c r="D64" s="0" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="E64" s="0" t="inlineStr">
         <is>
           <t>G8113</t>
         </is>
       </c>
-      <c r="F64" t="inlineStr">
-        <is>
-          <t>Del</t>
-        </is>
-      </c>
-      <c r="G64" t="inlineStr">
-        <is>
-          <t>Blr</t>
-        </is>
-      </c>
-      <c r="H64" t="inlineStr">
+      <c r="F64" s="0" t="inlineStr">
+        <is>
+          <t>DEL</t>
+        </is>
+      </c>
+      <c r="G64" s="0" t="inlineStr">
+        <is>
+          <t>BLR</t>
+        </is>
+      </c>
+      <c r="H64" s="0" t="inlineStr">
         <is>
           <t>0550</t>
         </is>
       </c>
     </row>
     <row r="65">
-      <c r="A65" t="inlineStr">
+      <c r="A65" s="0" t="inlineStr">
         <is>
           <t>f64</t>
         </is>
       </c>
-      <c r="B65" t="inlineStr">
+      <c r="B65" s="0" t="inlineStr">
         <is>
           <t>2019-11-07</t>
         </is>
       </c>
-      <c r="C65" t="inlineStr">
+      <c r="C65" s="0" t="inlineStr">
         <is>
           <t>Thu</t>
         </is>
       </c>
-      <c r="D65" t="inlineStr">
-        <is>
-          <t>Normal</t>
-        </is>
-      </c>
-      <c r="E65" t="inlineStr">
+      <c r="D65" s="0" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="E65" s="0" t="inlineStr">
         <is>
           <t>AI803</t>
         </is>
       </c>
-      <c r="F65" t="inlineStr">
-        <is>
-          <t>Del</t>
-        </is>
-      </c>
-      <c r="G65" t="inlineStr">
-        <is>
-          <t>Blr</t>
-        </is>
-      </c>
-      <c r="H65" t="inlineStr">
+      <c r="F65" s="0" t="inlineStr">
+        <is>
+          <t>DEL</t>
+        </is>
+      </c>
+      <c r="G65" s="0" t="inlineStr">
+        <is>
+          <t>BLR</t>
+        </is>
+      </c>
+      <c r="H65" s="0" t="inlineStr">
         <is>
           <t>0610</t>
         </is>

</xml_diff>

<commit_message>
Prices are going to excel file directly
</commit_message>
<xml_diff>
--- a/flights.xlsx
+++ b/flights.xlsx
@@ -262,12 +262,12 @@
     <row r="1">
       <c r="A1" s="0" t="inlineStr">
         <is>
-          <t>~ID</t>
+          <t>ID</t>
         </is>
       </c>
       <c r="B1" s="0" t="inlineStr">
         <is>
-          <t>~Date</t>
+          <t>Date</t>
         </is>
       </c>
       <c r="C1" s="0" t="inlineStr">
@@ -292,12 +292,12 @@
       </c>
       <c r="G1" s="0" t="inlineStr">
         <is>
-          <t>~To</t>
+          <t>To</t>
         </is>
       </c>
       <c r="H1" s="0" t="inlineStr">
         <is>
-          <t>~Dep Time</t>
+          <t>Dep Time</t>
         </is>
       </c>
     </row>

</xml_diff>